<commit_message>
Manca salvare il file
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaboldetti/Documents/GitHub/My_first_Repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D2E7EE-BC68-7D47-BA5A-CD005305BD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE6CF27-0386-9247-8BDE-6CBA8379697E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,8 +434,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>9.81</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -443,8 +442,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>19.62</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -452,8 +450,7 @@
         <v>3</v>
       </c>
       <c r="F7">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>29.43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -461,8 +458,7 @@
         <v>4</v>
       </c>
       <c r="F8">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>39.24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -470,8 +466,7 @@
         <v>5</v>
       </c>
       <c r="F9">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>49.050000000000004</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -479,8 +474,7 @@
         <v>6</v>
       </c>
       <c r="F10">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>58.86</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -488,8 +482,7 @@
         <v>7</v>
       </c>
       <c r="F11">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>68.67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -497,8 +490,7 @@
         <v>8</v>
       </c>
       <c r="F12">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>78.48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -506,8 +498,7 @@
         <v>9</v>
       </c>
       <c r="F13">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>88.29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -515,8 +506,7 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>98.100000000000009</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -524,8 +514,7 @@
         <v>11</v>
       </c>
       <c r="F15">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>107.91000000000001</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -533,8 +522,7 @@
         <v>12</v>
       </c>
       <c r="F16">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>117.72</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.2">
@@ -542,8 +530,7 @@
         <v>13</v>
       </c>
       <c r="F17">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>127.53</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.2">
@@ -551,8 +538,7 @@
         <v>14</v>
       </c>
       <c r="F18">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>137.34</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.2">
@@ -560,8 +546,7 @@
         <v>15</v>
       </c>
       <c r="F19">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>147.15</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.2">
@@ -569,8 +554,7 @@
         <v>16</v>
       </c>
       <c r="F20">
-        <f>Table1[[#This Row],[mass]]*9.81</f>
-        <v>156.96</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed path and avoided taking formulas as input
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -457,7 +457,7 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="10.5" customWidth="1" min="4" max="12"/>
   </cols>
@@ -515,9 +515,8 @@
       <c r="J6" t="n">
         <v>1</v>
       </c>
-      <c r="K6">
-        <f>RADIANS(H6)</f>
-        <v/>
+      <c r="K6" t="n">
+        <v>0.1919862177193762</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -536,9 +535,8 @@
       <c r="J7" t="n">
         <v>2</v>
       </c>
-      <c r="K7">
-        <f>RADIANS(H7)</f>
-        <v/>
+      <c r="K7" t="n">
+        <v>0.2268928027592629</v>
       </c>
       <c r="L7" t="n">
         <v>1</v>
@@ -557,9 +555,8 @@
       <c r="J8" t="n">
         <v>3</v>
       </c>
-      <c r="K8">
-        <f>RADIANS(H8)</f>
-        <v/>
+      <c r="K8" t="n">
+        <v>0.2443460952792061</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -578,9 +575,8 @@
       <c r="J9" t="n">
         <v>4</v>
       </c>
-      <c r="K9">
-        <f>RADIANS(H9)</f>
-        <v/>
+      <c r="K9" t="n">
+        <v>0.296705972839036</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -599,9 +595,8 @@
       <c r="J10" t="n">
         <v>5</v>
       </c>
-      <c r="K10">
-        <f>RADIANS(H10)</f>
-        <v/>
+      <c r="K10" t="n">
+        <v>0.3490658503988659</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -620,9 +615,8 @@
       <c r="J11" t="n">
         <v>6</v>
       </c>
-      <c r="K11">
-        <f>RADIANS(H11)</f>
-        <v/>
+      <c r="K11" t="n">
+        <v>0.4188790204786391</v>
       </c>
       <c r="L11" t="n">
         <v>1</v>
@@ -641,9 +635,8 @@
       <c r="J12" t="n">
         <v>7</v>
       </c>
-      <c r="K12">
-        <f>RADIANS(H12)</f>
-        <v/>
+      <c r="K12" t="n">
+        <v>0.471238898038469</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -662,9 +655,8 @@
       <c r="J13" t="n">
         <v>8</v>
       </c>
-      <c r="K13">
-        <f>RADIANS(H13)</f>
-        <v/>
+      <c r="K13" t="n">
+        <v>0.5235987755982988</v>
       </c>
       <c r="L13" t="n">
         <v>3</v>
@@ -683,9 +675,8 @@
       <c r="J14" t="n">
         <v>9</v>
       </c>
-      <c r="K14">
-        <f>RADIANS(H14)</f>
-        <v/>
+      <c r="K14" t="n">
+        <v>0.5759586531581288</v>
       </c>
       <c r="L14" t="n">
         <v>2</v>
@@ -704,9 +695,8 @@
       <c r="J15" t="n">
         <v>10</v>
       </c>
-      <c r="K15">
-        <f>RADIANS(H15)</f>
-        <v/>
+      <c r="K15" t="n">
+        <v>0.6108652381980153</v>
       </c>
       <c r="L15" t="n">
         <v>1</v>
@@ -725,9 +715,8 @@
       <c r="J16" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="K16">
-        <f>RADIANS(H16)</f>
-        <v/>
+      <c r="K16" t="n">
+        <v>0.6632251157578453</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -746,9 +735,8 @@
       <c r="J17" t="n">
         <v>12</v>
       </c>
-      <c r="K17">
-        <f>RADIANS(H17)</f>
-        <v/>
+      <c r="K17" t="n">
+        <v>0.7155849933176751</v>
       </c>
       <c r="L17" t="n">
         <v>4</v>
@@ -767,9 +755,8 @@
       <c r="J18" t="n">
         <v>13</v>
       </c>
-      <c r="K18">
-        <f>RADIANS(H18)</f>
-        <v/>
+      <c r="K18" t="n">
+        <v>0.767944870877505</v>
       </c>
       <c r="L18" t="n">
         <v>3</v>
@@ -788,9 +775,8 @@
       <c r="J19" t="n">
         <v>14</v>
       </c>
-      <c r="K19">
-        <f>RADIANS(H19)</f>
-        <v/>
+      <c r="K19" t="n">
+        <v>0.8203047484373349</v>
       </c>
       <c r="L19" t="n">
         <v>2</v>
@@ -809,9 +795,8 @@
       <c r="J20" t="n">
         <v>15</v>
       </c>
-      <c r="K20">
-        <f>RADIANS(H20)</f>
-        <v/>
+      <c r="K20" t="n">
+        <v>0.8726646259971648</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -832,7 +817,7 @@
         </is>
       </c>
       <c r="K23" t="n">
-        <v>54.097</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="24">
@@ -853,7 +838,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>9.963 + 0.092</t>
+          <t>0.049 + 0.092</t>
         </is>
       </c>
     </row>
@@ -875,7 +860,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2.662 + 0.637</t>
+          <t>0.119 + 0.637</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed issue with big tables
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -809,7 +809,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>234.94</v>
+        <v>939.7619999999999</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -828,7 +828,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>9.826 + 0.108</t>
+          <t>9.826 + 0.054</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>-7.225 + 1.049</t>
+          <t>-7.225 + 0.524</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">

</xml_diff>